<commit_message>
Updated data type for tabular data. Added System1 invoke app and close app workflows.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/valerie_gutierrez_uipath_com/Documents/Documents/UiPath/CalculateClientSecurityHash-REF-ACME/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6AEA7B0-9D31-4841-878B-32E0B5ED8DE2}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3D6570E-4292-4797-95B6-A39C3D5DB2C7}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>CalculateClientSecurityHash-REF-ACME</t>
+  </si>
+  <si>
+    <t>Name of asset in orchestrator</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -626,6 +629,9 @@
       </c>
       <c r="B6" t="s">
         <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
issue with same number being entered
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/valerie_gutierrez_uipath_com/Documents/Documents/UiPath/CalculateClientSecurityHash-REF-ACME/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3D6570E-4292-4797-95B6-A39C3D5DB2C7}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C30517CB-B730-434B-A126-A2CBD5BBFB74}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -550,7 +550,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>